<commit_message>
add models tableRegion and RateHighConsumption
</commit_message>
<xml_diff>
--- a/easylight/doc/table_rate.xlsx
+++ b/easylight/doc/table_rate.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
-    <t>namre_rate</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name_rate</t>
   </si>
   <si>
     <t>kilowatt</t>
@@ -91,7 +94,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -119,6 +122,21 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -138,6 +156,21 @@
       </right>
       <top style="thin">
         <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -180,7 +213,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -190,19 +223,25 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1287,17 +1326,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+      <pane topLeftCell="C2" xSplit="2" ySplit="1" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1307,60 +1347,84 @@
       <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" ht="20.15" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5">
         <v>250</v>
       </c>
     </row>
     <row r="3" ht="19.95" customHeight="1">
-      <c r="A3" t="s" s="5">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8">
         <v>300</v>
       </c>
     </row>
     <row r="4" ht="19.95" customHeight="1">
-      <c r="A4" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8">
         <v>400</v>
       </c>
     </row>
     <row r="5" ht="19.95" customHeight="1">
-      <c r="A5" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8">
         <v>850</v>
       </c>
     </row>
     <row r="6" ht="19.95" customHeight="1">
-      <c r="A6" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9">
         <v>1000</v>
       </c>
     </row>
     <row r="7" ht="19.95" customHeight="1">
-      <c r="A7" t="s" s="5">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9">
         <v>2000</v>
       </c>
     </row>
     <row r="8" ht="19.95" customHeight="1">
-      <c r="A8" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C8" s="9">
         <v>2500</v>
       </c>
     </row>

</xml_diff>